<commit_message>
Rows added in excel.
</commit_message>
<xml_diff>
--- a/src/main/resources/poidata/becon-data.xlsx
+++ b/src/main/resources/poidata/becon-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
   <si>
     <t>uuid</t>
   </si>
@@ -82,13 +82,24 @@
   </si>
   <si>
     <t>123</t>
+  </si>
+  <si>
+    <t>b9407f30-f5f8-466e-aff9-25556b57fe6d</t>
+  </si>
+  <si>
+    <t>St.Loius Airport shuttle 1</t>
+  </si>
+  <si>
+    <t>50765cb7-d9ea-4e21-99a4-fa879613a492</t>
+  </si>
+  <si>
+    <t>St.Loius Airport shuttle 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,10 +129,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -424,13 +438,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -596,7 +615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -619,7 +638,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -640,6 +659,52 @@
       </c>
       <c r="G11" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2">
+        <v>10345</v>
+      </c>
+      <c r="C12" s="2">
+        <v>19843</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2">
+        <v>123.5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>206</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2">
+        <v>62477</v>
+      </c>
+      <c r="C13" s="2">
+        <v>47058</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2">
+        <v>109.5</v>
+      </c>
+      <c r="F13" s="2">
+        <v>200</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added latitude and longitude to response
</commit_message>
<xml_diff>
--- a/src/main/resources/poidata/becon-data.xlsx
+++ b/src/main/resources/poidata/becon-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="30">
   <si>
     <t>uuid</t>
   </si>
@@ -141,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -151,6 +151,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -457,7 +460,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,11 +693,11 @@
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="4">
-        <v>123.5</v>
-      </c>
-      <c r="F12" s="4">
-        <v>206</v>
+      <c r="E12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>25</v>
@@ -713,11 +716,11 @@
       <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="4">
-        <v>109.5</v>
-      </c>
-      <c r="F13" s="4">
-        <v>200</v>
+      <c r="E13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>29</v>

</xml_diff>